<commit_message>
neuer Versuch mit Dictionaries in Listen
</commit_message>
<xml_diff>
--- a/BR New Game Blank.xlsx
+++ b/BR New Game Blank.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+  <si>
+    <t xml:space="preserve">Tag </t>
+  </si>
   <si>
     <t xml:space="preserve">Person</t>
   </si>
@@ -61,7 +64,7 @@
     <t xml:space="preserve">Verrät dir, ob du Rep bist gg. Mord</t>
   </si>
   <si>
-    <t xml:space="preserve">Rep Vorarbeiter </t>
+    <t xml:space="preserve">Rep Vorarbeiter</t>
   </si>
   <si>
     <t xml:space="preserve">Kippel</t>
@@ -70,7 +73,7 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Chefinsp. Bryant</t>
+    <t xml:space="preserve">Chefinspektor Bryant</t>
   </si>
   <si>
     <t xml:space="preserve">Polizeipräsidium</t>
@@ -82,38 +85,38 @@
     <t xml:space="preserve">Nur ID</t>
   </si>
   <si>
-    <t xml:space="preserve">2 Insp. Resch</t>
+    <t xml:space="preserve">Inspektor Resch</t>
   </si>
   <si>
     <t xml:space="preserve">Vk Tests ab Tag 4 (gefährlich!)</t>
   </si>
   <si>
-    <t xml:space="preserve">3 Insp. Steele</t>
+    <t xml:space="preserve">Inspektorin Steele</t>
   </si>
   <si>
     <t xml:space="preserve">Koordiniert Razzien</t>
   </si>
   <si>
-    <t xml:space="preserve">4 Insp. Mc Coy</t>
+    <t xml:space="preserve">Inspektor Mc Coy</t>
   </si>
   <si>
     <t xml:space="preserve">Nach verdeckten Tötungen:
 1 graues Indiz</t>
   </si>
   <si>
-    <t xml:space="preserve">5 Gerichtsmed.</t>
+    <t xml:space="preserve">Gerichtsmedizinerin</t>
   </si>
   <si>
     <t xml:space="preserve">Führt Autopsien durch</t>
   </si>
   <si>
-    <t xml:space="preserve">6 Wachoffizier</t>
+    <t xml:space="preserve">Wachoffizier</t>
   </si>
   <si>
     <t xml:space="preserve">Überwacht Büros</t>
   </si>
   <si>
-    <t xml:space="preserve">7 Howie Lee</t>
+    <t xml:space="preserve">Howie Lee</t>
   </si>
   <si>
     <t xml:space="preserve">Chinatown</t>
@@ -122,31 +125,31 @@
     <t xml:space="preserve">Gratis zufälliges Indiz</t>
   </si>
   <si>
-    <t xml:space="preserve">8 Mama Isabella</t>
+    <t xml:space="preserve">Mama Isabella</t>
   </si>
   <si>
     <t xml:space="preserve">Animoid Row</t>
   </si>
   <si>
-    <t xml:space="preserve">9 Early Q</t>
+    <t xml:space="preserve">Early Q</t>
   </si>
   <si>
     <t xml:space="preserve">Nichtclub Row</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Taffy Lewis</t>
+    <t xml:space="preserve">Taffy Lewis</t>
   </si>
   <si>
     <t xml:space="preserve">Hysteria Hall</t>
   </si>
   <si>
-    <t xml:space="preserve">11 Mia</t>
+    <t xml:space="preserve">Mia</t>
   </si>
   <si>
     <t xml:space="preserve">Gardner Strait</t>
   </si>
   <si>
-    <t xml:space="preserve">12 Crazy Legs Larry</t>
+    <t xml:space="preserve">Crazy Legs Larry</t>
   </si>
   <si>
     <t xml:space="preserve">Fahrzeughändler</t>
@@ -155,22 +158,22 @@
     <t xml:space="preserve">Ja stadt 1</t>
   </si>
   <si>
-    <t xml:space="preserve">13 Izo</t>
+    <t xml:space="preserve">Izo</t>
   </si>
   <si>
     <t xml:space="preserve">Händler (Ausrüstungskarten)</t>
   </si>
   <si>
-    <t xml:space="preserve">14 Bob Gorsky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 Emil Runciter</t>
+    <t xml:space="preserve">Bob Gorsky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emil Runciter</t>
   </si>
   <si>
     <t xml:space="preserve">Tierhändler</t>
   </si>
   <si>
-    <t xml:space="preserve">16 Slater</t>
+    <t xml:space="preserve">Slater</t>
   </si>
   <si>
     <t xml:space="preserve">Dieb</t>
@@ -179,61 +182,61 @@
     <t xml:space="preserve">Ja stadt</t>
   </si>
   <si>
-    <t xml:space="preserve">17 Arthur Kaufmann</t>
+    <t xml:space="preserve">Arthur Kaufmann</t>
   </si>
   <si>
     <t xml:space="preserve">Bombenleger</t>
   </si>
   <si>
-    <t xml:space="preserve">18 Rajesh Singh</t>
+    <t xml:space="preserve">Rajesh Singh</t>
   </si>
   <si>
     <t xml:space="preserve">Auftragsmörder</t>
   </si>
   <si>
-    <t xml:space="preserve">19 Dektora</t>
+    <t xml:space="preserve">Dektora</t>
   </si>
   <si>
     <t xml:space="preserve">2 Zufällige Indizien gegen Geld</t>
   </si>
   <si>
-    <t xml:space="preserve">20 Chiara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 Chalisa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 Gaff</t>
+    <t xml:space="preserve">Chiara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chalisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaff</t>
   </si>
   <si>
     <t xml:space="preserve">Gratis graues Indiz</t>
   </si>
   <si>
-    <t xml:space="preserve">23 George Gleason</t>
+    <t xml:space="preserve">George Gleason</t>
   </si>
   <si>
     <t xml:space="preserve">Spezifisches Indiz gegen Geld</t>
   </si>
   <si>
-    <t xml:space="preserve">24 Cash Grigorian</t>
+    <t xml:space="preserve">Cash Grigorian</t>
   </si>
   <si>
     <t xml:space="preserve">Hilft Reps</t>
   </si>
   <si>
-    <t xml:space="preserve">25 Willbur Mercer</t>
+    <t xml:space="preserve">Willbur Mercer</t>
   </si>
   <si>
     <t xml:space="preserve">Verschiedenes</t>
   </si>
   <si>
-    <t xml:space="preserve">26 Rick Deckard </t>
+    <t xml:space="preserve">Rick Deckard</t>
   </si>
   <si>
     <t xml:space="preserve">Verrät dir, ob du Rep bist (gratis)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja wohnundkip</t>
+    <t xml:space="preserve">Ja wohn+kip</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -266,22 +269,17 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -390,80 +388,76 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -544,448 +538,454 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="D7" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="7" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="E8" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="E9" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="E10" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>19</v>
+      <c r="E12" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14" t="s">
+      <c r="D17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+      <c r="E19" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16" t="s">
+      <c r="E21" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16" t="s">
+      <c r="E23" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16" t="s">
+      <c r="E24" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="s">
+      <c r="E25" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="s">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16" t="s">
+      <c r="E28" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16" t="s">
+      <c r="E29" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16" t="s">
+      <c r="E30" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18" t="s">
+      <c r="E31" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17" t="s">
         <v>70</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>